<commit_message>
changed the logic of the code
</commit_message>
<xml_diff>
--- a/Projects/CCNAYARMX/Comidas/Data/CCNayarTemplate2020-Fondas Rsr.xlsx
+++ b/Projects/CCNAYARMX/Comidas/Data/CCNayarTemplate2020-Fondas Rsr.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="167">
   <si>
     <t xml:space="preserve">KPI Number</t>
   </si>
@@ -309,9 +309,6 @@
   </si>
   <si>
     <t xml:space="preserve">store_fk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Task/ Template Group</t>
   </si>
   <si>
     <t xml:space="preserve">store-type</t>
@@ -743,7 +740,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -776,14 +773,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -857,10 +846,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -983,20 +968,20 @@
   </sheetPr>
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.81781376518219"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0688259109312"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.9919028340081"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.6356275303644"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="57.9514170040486"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="58.914979757085"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="58.8097165991903"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="59.7732793522267"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.1417004048583"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.63967611336032"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.6032388663968"/>
@@ -1153,34 +1138,34 @@
       <c r="J5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="n">
+      <c r="A6" s="2" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="8" t="n">
+      <c r="C6" s="2" t="n">
         <v>60</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="8" t="s">
+      <c r="E6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="80" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="2" t="n">
@@ -1262,7 +1247,7 @@
         <v>34</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="8" t="s">
         <v>35</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -1292,7 +1277,7 @@
         <v>34</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="8" t="s">
         <v>39</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -1346,7 +1331,7 @@
         <v>41</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="8" t="s">
         <v>42</v>
       </c>
       <c r="E13" s="2" t="s">
@@ -1376,7 +1361,7 @@
         <v>41</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="8" t="s">
         <v>44</v>
       </c>
       <c r="E14" s="2" t="s">
@@ -1455,7 +1440,7 @@
       <c r="H16" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="I16" s="11" t="s">
+      <c r="I16" s="9" t="s">
         <v>53</v>
       </c>
       <c r="J16" s="5"/>
@@ -1479,7 +1464,7 @@
         <v>26</v>
       </c>
       <c r="H17" s="4"/>
-      <c r="I17" s="11"/>
+      <c r="I17" s="9"/>
       <c r="J17" s="5"/>
     </row>
   </sheetData>
@@ -1507,68 +1492,68 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.7408906882591"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.8097165991903"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.3846153846154"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="64.914979757085"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.3846153846154"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.4534412955466"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.8137651821862"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="65.9838056680162"/>
     <col collapsed="false" hidden="false" max="10" min="6" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="17.4615384615385"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="O1" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="P1" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="Q1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="R1" s="10" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1579,13 +1564,13 @@
       <c r="B2" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="11" t="s">
         <v>67</v>
       </c>
       <c r="F2" s="0" t="s">
@@ -1600,13 +1585,13 @@
       <c r="I2" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="J2" s="14" t="n">
+      <c r="J2" s="12" t="n">
         <v>2805</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="L2" s="16" t="n">
+      <c r="L2" s="14" t="n">
         <v>5</v>
       </c>
       <c r="M2" s="0" t="s">
@@ -1629,13 +1614,13 @@
       <c r="B3" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="11" t="s">
         <v>74</v>
       </c>
       <c r="F3" s="0" t="s">
@@ -1650,11 +1635,11 @@
       <c r="I3" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="K3" s="14"/>
-      <c r="L3" s="16" t="n">
+      <c r="K3" s="12"/>
+      <c r="L3" s="14" t="n">
         <v>2.5</v>
       </c>
       <c r="M3" s="0" t="s">
@@ -1677,13 +1662,13 @@
       <c r="B4" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="11" t="s">
         <v>67</v>
       </c>
       <c r="F4" s="0" t="s">
@@ -1698,13 +1683,13 @@
       <c r="I4" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="14" t="n">
+      <c r="J4" s="12" t="n">
         <v>2805</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="L4" s="16" t="n">
+      <c r="L4" s="14" t="n">
         <v>5</v>
       </c>
       <c r="M4" s="0" t="s">
@@ -1727,13 +1712,13 @@
       <c r="B5" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="11" t="s">
         <v>74</v>
       </c>
       <c r="F5" s="0" t="s">
@@ -1748,11 +1733,11 @@
       <c r="I5" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="J5" s="14" t="n">
+      <c r="J5" s="12" t="n">
         <v>2804</v>
       </c>
-      <c r="K5" s="14"/>
-      <c r="L5" s="16" t="n">
+      <c r="K5" s="12"/>
+      <c r="L5" s="14" t="n">
         <v>2.5</v>
       </c>
       <c r="M5" s="0" t="s">
@@ -1786,75 +1771,75 @@
   </sheetPr>
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.4898785425101"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.1336032388664"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="57.9514170040486"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="58.914979757085"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.748987854251"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.6761133603239"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="12" min="11" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="O1" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="P1" s="10" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1862,10 +1847,10 @@
       <c r="A2" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="8" t="s">
         <v>87</v>
       </c>
       <c r="D2" s="0" t="s">
@@ -1961,117 +1946,117 @@
   </sheetPr>
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.2429149797571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.8825910931174"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.6720647773279"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.7368421052632"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
+    <row r="1" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="G1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="J1" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="K1" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="L1" s="19" t="s">
+      <c r="M1" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="240" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="M1" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="N1" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="O1" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="P1" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q1" s="19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="240" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="22" t="s">
+      <c r="D2" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="24" t="s">
+      <c r="H2" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="J2" s="22"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="N2" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="O2" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="H2" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="I2" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="J2" s="24"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="M2" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="N2" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="O2" s="26" t="s">
-        <v>99</v>
-      </c>
-      <c r="P2" s="25" t="s">
+      <c r="P2" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" s="25" t="s">
+      <c r="Q2" s="23" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2100,43 +2085,43 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.3846153846154"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.8137651821862"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="46.4898785425101"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="47.1336032388664"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.2834008097166"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="I1" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="10" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2144,20 +2129,20 @@
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="15" t="s">
         <v>104</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>105</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>13</v>
@@ -2166,7 +2151,7 @@
         <v>22</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J2" s="0" t="s">
         <v>16</v>
@@ -2190,118 +2175,118 @@
   </sheetPr>
   <dimension ref="A1:AC8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0688259109312"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="89.5506072874494"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.2834008097166"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="25.9230769230769"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="15" min="10" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="91.1578947368421"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="15" min="10" style="0" width="12.9595141700405"/>
     <col collapsed="false" hidden="false" max="17" min="16" style="0" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="67.2712550607288"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="68.3400809716599"/>
     <col collapsed="false" hidden="false" max="22" min="20" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="20.4615384615385"/>
     <col collapsed="false" hidden="false" max="25" min="25" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="27" min="26" style="0" width="29.8866396761134"/>
+    <col collapsed="false" hidden="false" max="27" min="26" style="0" width="30.3157894736842"/>
     <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="J1" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="K1" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="K1" s="28" t="s">
+      <c r="L1" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="L1" s="28" t="s">
+      <c r="M1" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="M1" s="28" t="s">
+      <c r="N1" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="N1" s="28" t="s">
+      <c r="O1" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="P1" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="P1" s="28" t="s">
+      <c r="Q1" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="28" t="s">
+      <c r="R1" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="R1" s="28" t="s">
+      <c r="S1" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="S1" s="28" t="s">
+      <c r="T1" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="T1" s="28" t="s">
+      <c r="U1" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="U1" s="28" t="s">
+      <c r="V1" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="V1" s="28" t="s">
+      <c r="W1" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="W1" s="28" t="s">
+      <c r="X1" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="X1" s="28" t="s">
+      <c r="Y1" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="Y1" s="28" t="s">
+      <c r="Z1" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="Z1" s="28" t="s">
+      <c r="AA1" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="AA1" s="28" t="s">
+      <c r="AB1" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="AB1" s="28" t="s">
+      <c r="AC1" s="26" t="s">
         <v>127</v>
-      </c>
-      <c r="AC1" s="28" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2318,52 +2303,52 @@
         <v>28</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="J2" s="27" t="s">
         <v>132</v>
-      </c>
-      <c r="J2" s="30" t="s">
-        <v>133</v>
       </c>
       <c r="K2" s="0" t="n">
         <v>245</v>
       </c>
-      <c r="L2" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="M2" s="31" t="s">
+      <c r="L2" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="M2" s="28" t="s">
         <v>92</v>
       </c>
       <c r="N2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O2" s="32" t="s">
-        <v>135</v>
+      <c r="O2" s="29" t="s">
+        <v>134</v>
       </c>
       <c r="P2" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="Q2" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="R2" s="33" t="s">
+      <c r="Q2" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="R2" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="S2" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="S2" s="34" t="s">
+      <c r="T2" s="0" t="s">
         <v>137</v>
-      </c>
-      <c r="T2" s="0" t="s">
-        <v>138</v>
       </c>
       <c r="U2" s="0" t="s">
         <v>70</v>
@@ -2375,22 +2360,22 @@
         <v>5</v>
       </c>
       <c r="X2" s="0" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Y2" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="Z2" s="34" t="s">
+      <c r="Z2" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="AA2" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="AA2" s="34" t="s">
+      <c r="AB2" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="AB2" s="34" t="s">
+      <c r="AC2" s="0" t="s">
         <v>141</v>
-      </c>
-      <c r="AC2" s="0" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2407,52 +2392,52 @@
         <v>28</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="I3" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="J3" s="30" t="s">
-        <v>133</v>
+      <c r="I3" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="J3" s="27" t="s">
+        <v>132</v>
       </c>
       <c r="K3" s="0" t="n">
         <v>245</v>
       </c>
-      <c r="L3" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="M3" s="31" t="s">
+      <c r="L3" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="M3" s="28" t="s">
         <v>92</v>
       </c>
       <c r="N3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O3" s="32" t="s">
-        <v>135</v>
+      <c r="O3" s="29" t="s">
+        <v>134</v>
       </c>
       <c r="P3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="Q3" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="R3" s="33" t="s">
+      <c r="Q3" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="R3" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="S3" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="S3" s="34" t="s">
+      <c r="T3" s="0" t="s">
         <v>137</v>
-      </c>
-      <c r="T3" s="0" t="s">
-        <v>138</v>
       </c>
       <c r="U3" s="0" t="s">
         <v>70</v>
@@ -2464,22 +2449,22 @@
         <v>4</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Y3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="Z3" s="34" t="s">
+      <c r="Z3" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="AA3" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="AA3" s="34" t="s">
+      <c r="AB3" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="AB3" s="34" t="s">
+      <c r="AC3" s="0" t="s">
         <v>141</v>
-      </c>
-      <c r="AC3" s="0" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2496,52 +2481,52 @@
         <v>28</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>130</v>
-      </c>
       <c r="G4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="I4" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="J4" s="30" t="s">
-        <v>133</v>
+      <c r="I4" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="J4" s="27" t="s">
+        <v>132</v>
       </c>
       <c r="K4" s="0" t="n">
         <v>245</v>
       </c>
-      <c r="L4" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="M4" s="31" t="s">
+      <c r="L4" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="M4" s="28" t="s">
         <v>92</v>
       </c>
       <c r="N4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O4" s="32" t="s">
-        <v>135</v>
+      <c r="O4" s="29" t="s">
+        <v>134</v>
       </c>
       <c r="P4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="Q4" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="R4" s="33" t="s">
+      <c r="Q4" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="R4" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="S4" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="S4" s="34" t="s">
+      <c r="T4" s="0" t="s">
         <v>137</v>
-      </c>
-      <c r="T4" s="0" t="s">
-        <v>138</v>
       </c>
       <c r="U4" s="0" t="s">
         <v>70</v>
@@ -2553,22 +2538,22 @@
         <v>4</v>
       </c>
       <c r="X4" s="0" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Y4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="Z4" s="34" t="s">
+      <c r="Z4" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="AA4" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="AA4" s="34" t="s">
+      <c r="AB4" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="AB4" s="34" t="s">
+      <c r="AC4" s="0" t="s">
         <v>141</v>
-      </c>
-      <c r="AC4" s="0" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2585,52 +2570,52 @@
         <v>28</v>
       </c>
       <c r="E5" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="I5" s="29" t="s">
-        <v>145</v>
-      </c>
-      <c r="J5" s="30" t="s">
-        <v>133</v>
+      <c r="I5" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="J5" s="27" t="s">
+        <v>132</v>
       </c>
       <c r="K5" s="0" t="n">
         <v>245</v>
       </c>
-      <c r="L5" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="M5" s="31" t="s">
+      <c r="L5" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="M5" s="28" t="s">
         <v>92</v>
       </c>
       <c r="N5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O5" s="32" t="s">
-        <v>135</v>
+      <c r="O5" s="29" t="s">
+        <v>134</v>
       </c>
       <c r="P5" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="Q5" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="R5" s="33" t="s">
+      <c r="Q5" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="R5" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="S5" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="S5" s="34" t="s">
+      <c r="T5" s="0" t="s">
         <v>137</v>
-      </c>
-      <c r="T5" s="0" t="s">
-        <v>138</v>
       </c>
       <c r="U5" s="0" t="s">
         <v>70</v>
@@ -2642,22 +2627,22 @@
         <v>3</v>
       </c>
       <c r="X5" s="0" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Y5" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="Z5" s="34" t="s">
+      <c r="Z5" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="AA5" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="AA5" s="34" t="s">
+      <c r="AB5" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="AB5" s="34" t="s">
+      <c r="AC5" s="0" t="s">
         <v>141</v>
-      </c>
-      <c r="AC5" s="0" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2674,52 +2659,52 @@
         <v>28</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>130</v>
-      </c>
       <c r="G6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H6" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="I6" s="29" t="s">
-        <v>145</v>
-      </c>
-      <c r="J6" s="30" t="s">
-        <v>133</v>
+      <c r="J6" s="27" t="s">
+        <v>132</v>
       </c>
       <c r="K6" s="0" t="n">
         <v>245</v>
       </c>
-      <c r="L6" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="M6" s="31" t="s">
+      <c r="L6" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="M6" s="28" t="s">
         <v>92</v>
       </c>
       <c r="N6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O6" s="32" t="s">
-        <v>135</v>
+      <c r="O6" s="29" t="s">
+        <v>134</v>
       </c>
       <c r="P6" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="Q6" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="R6" s="33" t="s">
+      <c r="Q6" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="R6" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="S6" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="S6" s="34" t="s">
+      <c r="T6" s="0" t="s">
         <v>137</v>
-      </c>
-      <c r="T6" s="0" t="s">
-        <v>138</v>
       </c>
       <c r="U6" s="0" t="s">
         <v>70</v>
@@ -2731,22 +2716,22 @@
         <v>3</v>
       </c>
       <c r="X6" s="0" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Y6" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="Z6" s="34" t="s">
+      <c r="Z6" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="AA6" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="AA6" s="34" t="s">
+      <c r="AB6" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="AB6" s="34" t="s">
+      <c r="AC6" s="0" t="s">
         <v>141</v>
-      </c>
-      <c r="AC6" s="0" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2763,52 +2748,52 @@
         <v>28</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="I7" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="J7" s="30" t="s">
-        <v>133</v>
+      <c r="I7" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="J7" s="27" t="s">
+        <v>132</v>
       </c>
       <c r="K7" s="0" t="n">
         <v>245</v>
       </c>
-      <c r="L7" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="M7" s="31" t="s">
+      <c r="L7" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="M7" s="28" t="s">
         <v>92</v>
       </c>
       <c r="N7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O7" s="32" t="s">
-        <v>135</v>
+      <c r="O7" s="29" t="s">
+        <v>134</v>
       </c>
       <c r="P7" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="Q7" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="R7" s="33" t="s">
+      <c r="Q7" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="R7" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="S7" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="S7" s="34" t="s">
+      <c r="T7" s="0" t="s">
         <v>137</v>
-      </c>
-      <c r="T7" s="0" t="s">
-        <v>138</v>
       </c>
       <c r="U7" s="0" t="s">
         <v>70</v>
@@ -2820,22 +2805,22 @@
         <v>2</v>
       </c>
       <c r="X7" s="0" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Y7" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="Z7" s="34" t="s">
+      <c r="Z7" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="AA7" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="AA7" s="34" t="s">
+      <c r="AB7" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="AB7" s="34" t="s">
+      <c r="AC7" s="0" t="s">
         <v>141</v>
-      </c>
-      <c r="AC7" s="0" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="48" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2852,52 +2837,52 @@
         <v>28</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>130</v>
-      </c>
       <c r="G8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="I8" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="J8" s="30" t="s">
-        <v>133</v>
+        <v>143</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="J8" s="27" t="s">
+        <v>132</v>
       </c>
       <c r="K8" s="0" t="n">
         <v>245</v>
       </c>
-      <c r="L8" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="M8" s="31" t="s">
+      <c r="L8" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="M8" s="28" t="s">
         <v>92</v>
       </c>
       <c r="N8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O8" s="32" t="s">
-        <v>135</v>
+      <c r="O8" s="29" t="s">
+        <v>134</v>
       </c>
       <c r="P8" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="Q8" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="R8" s="33" t="s">
+      <c r="Q8" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="R8" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="S8" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="S8" s="34" t="s">
+      <c r="T8" s="0" t="s">
         <v>137</v>
-      </c>
-      <c r="T8" s="0" t="s">
-        <v>138</v>
       </c>
       <c r="U8" s="0" t="s">
         <v>70</v>
@@ -2909,22 +2894,22 @@
         <v>2</v>
       </c>
       <c r="X8" s="0" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Y8" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="Z8" s="34" t="s">
+      <c r="Z8" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="AA8" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="AA8" s="34" t="s">
+      <c r="AB8" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="AB8" s="34" t="s">
+      <c r="AC8" s="0" t="s">
         <v>141</v>
-      </c>
-      <c r="AC8" s="0" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2946,17 +2931,17 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="5" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.17004048583"/>
     <col collapsed="false" hidden="false" max="8" min="7" style="0" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="10" min="9" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="13" min="11" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="32.9919028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -2979,41 +2964,41 @@
       <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="H1" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="I1" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="I1" s="35" t="s">
-        <v>110</v>
-      </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="K1" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="K1" s="35" t="s">
+      <c r="L1" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="M1" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="N1" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="O1" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="P1" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="L1" s="35" t="s">
-        <v>119</v>
-      </c>
-      <c r="M1" s="35" t="s">
-        <v>116</v>
-      </c>
-      <c r="N1" s="35" t="s">
-        <v>117</v>
-      </c>
-      <c r="O1" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="P1" s="35" t="s">
+      <c r="Q1" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="Q1" s="35" t="s">
-        <v>150</v>
-      </c>
-      <c r="R1" s="35" t="s">
-        <v>127</v>
+      <c r="R1" s="32" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="128" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3035,32 +3020,32 @@
       <c r="F2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="33" t="s">
         <v>88</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I2" s="0" t="s">
         <v>25</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K2" s="0" t="n">
         <v>80</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M2" s="0" t="s">
         <v>58</v>
       </c>
       <c r="N2" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>152</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>153</v>
       </c>
       <c r="P2" s="0" t="s">
         <v>92</v>
@@ -3097,48 +3082,48 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.4615384615385"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.9230769230769"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="32.6720647773279"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="38.7773279352227"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="33.1012145748988"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="39.4210526315789"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="I1" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="J1" s="35" t="s">
         <v>156</v>
-      </c>
-      <c r="J1" s="38" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3161,13 +3146,13 @@
         <v>26</v>
       </c>
       <c r="G2" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="H2" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="J2" s="0" t="s">
         <v>159</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="64" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3180,7 +3165,7 @@
       <c r="C3" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -3193,10 +3178,10 @@
         <v>28</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="J3" s="34" t="s">
-        <v>161</v>
+        <v>158</v>
+      </c>
+      <c r="J3" s="31" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="64" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3218,14 +3203,14 @@
       <c r="F4" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="34" t="s">
-        <v>162</v>
+      <c r="G4" s="31" t="s">
+        <v>161</v>
       </c>
       <c r="H4" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="J4" s="0" t="s">
         <v>159</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="68" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3247,14 +3232,14 @@
       <c r="F5" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="J5" s="36" t="s">
         <v>163</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="J5" s="39" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="68" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3276,14 +3261,14 @@
       <c r="F6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="10" t="s">
-        <v>165</v>
+      <c r="G6" s="8" t="s">
+        <v>164</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="J6" s="39" t="s">
-        <v>164</v>
+        <v>158</v>
+      </c>
+      <c r="J6" s="36" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="80" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3302,24 +3287,24 @@
       <c r="F7" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="34" t="s">
+      <c r="G7" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="J7" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="H7" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>167</v>
-      </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F12" s="10"/>
+      <c r="F12" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="10"/>
+      <c r="D14" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F20" s="8"/>
+      <c r="F20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F21" s="4"/>

</xml_diff>